<commit_message>
modified and added final dataset
</commit_message>
<xml_diff>
--- a/flipkart_categories.xlsx
+++ b/flipkart_categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\Desktop\setubhandhan\product price prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578940E2-EC8E-4D90-AED1-AF3EFA5D3CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A606C7B-3920-44FB-AC84-8AAE9C2CB422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2676" yWindow="2676" windowWidth="10128" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="url" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="860">
   <si>
     <t>Mobile Accessories</t>
   </si>
@@ -2769,7 +2769,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2787,7 +2787,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -3072,8 +3071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C299" workbookViewId="0">
-      <selection activeCell="D319" sqref="D319"/>
+    <sheetView tabSelected="1" topLeftCell="A308" workbookViewId="0">
+      <selection activeCell="A271" sqref="A271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5958,10 +5957,10 @@
       <c r="A206" t="s">
         <v>683</v>
       </c>
-      <c r="B206" s="9" t="s">
+      <c r="B206" t="s">
         <v>671</v>
       </c>
-      <c r="C206" s="9" t="s">
+      <c r="C206" t="s">
         <v>671</v>
       </c>
       <c r="D206" t="s">
@@ -5972,7 +5971,7 @@
       <c r="A207" t="s">
         <v>683</v>
       </c>
-      <c r="B207" s="9" t="s">
+      <c r="B207" t="s">
         <v>685</v>
       </c>
       <c r="C207" t="s">
@@ -5986,7 +5985,7 @@
       <c r="A208" t="s">
         <v>683</v>
       </c>
-      <c r="B208" s="9" t="s">
+      <c r="B208" t="s">
         <v>685</v>
       </c>
       <c r="C208" t="s">
@@ -6000,7 +5999,7 @@
       <c r="A209" t="s">
         <v>683</v>
       </c>
-      <c r="B209" s="9" t="s">
+      <c r="B209" t="s">
         <v>685</v>
       </c>
       <c r="C209" t="s">
@@ -6014,7 +6013,7 @@
       <c r="A210" t="s">
         <v>683</v>
       </c>
-      <c r="B210" s="9" t="s">
+      <c r="B210" t="s">
         <v>685</v>
       </c>
       <c r="C210" t="s">
@@ -6028,7 +6027,7 @@
       <c r="A211" t="s">
         <v>683</v>
       </c>
-      <c r="B211" s="9" t="s">
+      <c r="B211" t="s">
         <v>685</v>
       </c>
       <c r="C211" t="s">
@@ -6143,7 +6142,7 @@
       <c r="B219" t="s">
         <v>701</v>
       </c>
-      <c r="C219" s="10" t="s">
+      <c r="C219" s="9" t="s">
         <v>149</v>
       </c>
       <c r="D219" t="s">
@@ -6182,10 +6181,10 @@
       <c r="A222" t="s">
         <v>683</v>
       </c>
-      <c r="B222" s="9" t="s">
+      <c r="B222" t="s">
         <v>679</v>
       </c>
-      <c r="C222" s="9" t="s">
+      <c r="C222" t="s">
         <v>679</v>
       </c>
       <c r="D222" t="s">
@@ -6196,7 +6195,7 @@
       <c r="A223" t="s">
         <v>683</v>
       </c>
-      <c r="B223" s="9" t="s">
+      <c r="B223" t="s">
         <v>680</v>
       </c>
       <c r="C223" t="s">
@@ -6210,7 +6209,7 @@
       <c r="A224" t="s">
         <v>683</v>
       </c>
-      <c r="B224" s="9" t="s">
+      <c r="B224" t="s">
         <v>680</v>
       </c>
       <c r="C224" t="s">
@@ -6252,10 +6251,10 @@
       <c r="A227" t="s">
         <v>683</v>
       </c>
-      <c r="B227" s="9" t="s">
+      <c r="B227" t="s">
         <v>711</v>
       </c>
-      <c r="C227" s="9" t="s">
+      <c r="C227" t="s">
         <v>711</v>
       </c>
       <c r="D227" t="s">
@@ -6266,10 +6265,10 @@
       <c r="A228" t="s">
         <v>683</v>
       </c>
-      <c r="B228" s="9" t="s">
+      <c r="B228" t="s">
         <v>712</v>
       </c>
-      <c r="C228" s="9" t="s">
+      <c r="C228" t="s">
         <v>712</v>
       </c>
       <c r="D228" t="s">
@@ -6280,10 +6279,10 @@
       <c r="A229" t="s">
         <v>683</v>
       </c>
-      <c r="B229" s="9" t="s">
+      <c r="B229" t="s">
         <v>713</v>
       </c>
-      <c r="C229" s="9" t="s">
+      <c r="C229" t="s">
         <v>713</v>
       </c>
       <c r="D229" t="s">
@@ -6294,7 +6293,7 @@
       <c r="A230" t="s">
         <v>683</v>
       </c>
-      <c r="B230" s="9" t="s">
+      <c r="B230" t="s">
         <v>719</v>
       </c>
       <c r="C230" t="s">
@@ -6308,7 +6307,7 @@
       <c r="A231" t="s">
         <v>683</v>
       </c>
-      <c r="B231" s="9" t="s">
+      <c r="B231" t="s">
         <v>719</v>
       </c>
       <c r="C231" t="s">
@@ -6798,7 +6797,7 @@
       <c r="A266" t="s">
         <v>802</v>
       </c>
-      <c r="B266" s="9" t="s">
+      <c r="B266" t="s">
         <v>777</v>
       </c>
       <c r="C266" t="s">
@@ -6809,6 +6808,12 @@
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>802</v>
+      </c>
+      <c r="B267" t="s">
+        <v>777</v>
+      </c>
       <c r="C267" t="s">
         <v>284</v>
       </c>
@@ -6817,6 +6822,12 @@
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>802</v>
+      </c>
+      <c r="B268" t="s">
+        <v>777</v>
+      </c>
       <c r="C268" t="s">
         <v>288</v>
       </c>
@@ -6825,6 +6836,12 @@
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>802</v>
+      </c>
+      <c r="B269" t="s">
+        <v>777</v>
+      </c>
       <c r="C269" t="s">
         <v>292</v>
       </c>
@@ -6833,6 +6850,12 @@
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>802</v>
+      </c>
+      <c r="B270" t="s">
+        <v>777</v>
+      </c>
       <c r="C270" t="s">
         <v>296</v>
       </c>
@@ -6841,7 +6864,10 @@
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B271" s="9" t="s">
+      <c r="A271" t="s">
+        <v>802</v>
+      </c>
+      <c r="B271" t="s">
         <v>775</v>
       </c>
       <c r="C271" t="s">
@@ -6852,6 +6878,12 @@
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>802</v>
+      </c>
+      <c r="B272" t="s">
+        <v>775</v>
+      </c>
       <c r="C272" t="s">
         <v>298</v>
       </c>
@@ -6859,7 +6891,13 @@
         <v>809</v>
       </c>
     </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>802</v>
+      </c>
+      <c r="B273" t="s">
+        <v>775</v>
+      </c>
       <c r="C273" t="s">
         <v>301</v>
       </c>
@@ -6867,8 +6905,11 @@
         <v>810</v>
       </c>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B274" s="9" t="s">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>802</v>
+      </c>
+      <c r="B274" t="s">
         <v>778</v>
       </c>
       <c r="C274" t="s">
@@ -6878,7 +6919,13 @@
         <v>811</v>
       </c>
     </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>802</v>
+      </c>
+      <c r="B275" t="s">
+        <v>778</v>
+      </c>
       <c r="C275" t="s">
         <v>311</v>
       </c>
@@ -6886,7 +6933,13 @@
         <v>812</v>
       </c>
     </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>802</v>
+      </c>
+      <c r="B276" t="s">
+        <v>778</v>
+      </c>
       <c r="C276" t="s">
         <v>312</v>
       </c>
@@ -6894,7 +6947,13 @@
         <v>813</v>
       </c>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>802</v>
+      </c>
+      <c r="B277" t="s">
+        <v>778</v>
+      </c>
       <c r="C277" t="s">
         <v>314</v>
       </c>
@@ -6902,7 +6961,13 @@
         <v>814</v>
       </c>
     </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>802</v>
+      </c>
+      <c r="B278" t="s">
+        <v>778</v>
+      </c>
       <c r="C278" t="s">
         <v>317</v>
       </c>
@@ -6910,7 +6975,10 @@
         <v>815</v>
       </c>
     </row>
-    <row r="279" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>802</v>
+      </c>
       <c r="B279" t="s">
         <v>779</v>
       </c>
@@ -6921,7 +6989,10 @@
         <v>816</v>
       </c>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>802</v>
+      </c>
       <c r="B280" t="s">
         <v>782</v>
       </c>
@@ -6932,7 +7003,13 @@
         <v>818</v>
       </c>
     </row>
-    <row r="281" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>802</v>
+      </c>
+      <c r="B281" t="s">
+        <v>782</v>
+      </c>
       <c r="C281" t="s">
         <v>289</v>
       </c>
@@ -6940,7 +7017,13 @@
         <v>819</v>
       </c>
     </row>
-    <row r="282" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>802</v>
+      </c>
+      <c r="B282" t="s">
+        <v>782</v>
+      </c>
       <c r="C282" t="s">
         <v>293</v>
       </c>
@@ -6948,7 +7031,10 @@
         <v>820</v>
       </c>
     </row>
-    <row r="283" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>802</v>
+      </c>
       <c r="B283" t="s">
         <v>783</v>
       </c>
@@ -6959,7 +7045,13 @@
         <v>821</v>
       </c>
     </row>
-    <row r="284" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>802</v>
+      </c>
+      <c r="B284" t="s">
+        <v>783</v>
+      </c>
       <c r="C284" t="s">
         <v>781</v>
       </c>
@@ -6967,7 +7059,13 @@
         <v>822</v>
       </c>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>802</v>
+      </c>
+      <c r="B285" t="s">
+        <v>783</v>
+      </c>
       <c r="C285" t="s">
         <v>299</v>
       </c>
@@ -6975,7 +7073,13 @@
         <v>823</v>
       </c>
     </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>802</v>
+      </c>
+      <c r="B286" t="s">
+        <v>783</v>
+      </c>
       <c r="C286" t="s">
         <v>784</v>
       </c>
@@ -6983,7 +7087,13 @@
         <v>824</v>
       </c>
     </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>802</v>
+      </c>
+      <c r="B287" t="s">
+        <v>783</v>
+      </c>
       <c r="C287" t="s">
         <v>304</v>
       </c>
@@ -6991,7 +7101,13 @@
         <v>825</v>
       </c>
     </row>
-    <row r="288" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>802</v>
+      </c>
+      <c r="B288" t="s">
+        <v>783</v>
+      </c>
       <c r="C288" t="s">
         <v>308</v>
       </c>
@@ -6999,7 +7115,10 @@
         <v>826</v>
       </c>
     </row>
-    <row r="289" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>802</v>
+      </c>
       <c r="B289" t="s">
         <v>785</v>
       </c>
@@ -7010,7 +7129,10 @@
         <v>827</v>
       </c>
     </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>802</v>
+      </c>
       <c r="B290" t="s">
         <v>817</v>
       </c>
@@ -7021,7 +7143,13 @@
         <v>828</v>
       </c>
     </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>802</v>
+      </c>
+      <c r="B291" t="s">
+        <v>817</v>
+      </c>
       <c r="C291" t="s">
         <v>320</v>
       </c>
@@ -7029,7 +7157,10 @@
         <v>829</v>
       </c>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>802</v>
+      </c>
       <c r="B292" t="s">
         <v>830</v>
       </c>
@@ -7040,7 +7171,13 @@
         <v>832</v>
       </c>
     </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>802</v>
+      </c>
+      <c r="B293" t="s">
+        <v>830</v>
+      </c>
       <c r="C293" t="s">
         <v>286</v>
       </c>
@@ -7048,7 +7185,13 @@
         <v>833</v>
       </c>
     </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>802</v>
+      </c>
+      <c r="B294" t="s">
+        <v>830</v>
+      </c>
       <c r="C294" t="s">
         <v>835</v>
       </c>
@@ -7056,7 +7199,13 @@
         <v>834</v>
       </c>
     </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>802</v>
+      </c>
+      <c r="B295" t="s">
+        <v>830</v>
+      </c>
       <c r="C295" t="s">
         <v>294</v>
       </c>
@@ -7064,7 +7213,13 @@
         <v>836</v>
       </c>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>802</v>
+      </c>
+      <c r="B296" t="s">
+        <v>830</v>
+      </c>
       <c r="C296" t="s">
         <v>297</v>
       </c>
@@ -7072,7 +7227,13 @@
         <v>837</v>
       </c>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>802</v>
+      </c>
+      <c r="B297" t="s">
+        <v>830</v>
+      </c>
       <c r="C297" t="s">
         <v>787</v>
       </c>
@@ -7080,7 +7241,13 @@
         <v>838</v>
       </c>
     </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>802</v>
+      </c>
+      <c r="B298" t="s">
+        <v>830</v>
+      </c>
       <c r="C298" t="s">
         <v>786</v>
       </c>
@@ -7088,7 +7255,10 @@
         <v>839</v>
       </c>
     </row>
-    <row r="299" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>802</v>
+      </c>
       <c r="B299" t="s">
         <v>21</v>
       </c>
@@ -7099,7 +7269,13 @@
         <v>840</v>
       </c>
     </row>
-    <row r="300" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>802</v>
+      </c>
+      <c r="B300" t="s">
+        <v>21</v>
+      </c>
       <c r="C300" t="s">
         <v>305</v>
       </c>
@@ -7107,7 +7283,10 @@
         <v>841</v>
       </c>
     </row>
-    <row r="301" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>802</v>
+      </c>
       <c r="B301" t="s">
         <v>831</v>
       </c>
@@ -7118,7 +7297,13 @@
         <v>842</v>
       </c>
     </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>802</v>
+      </c>
+      <c r="B302" t="s">
+        <v>831</v>
+      </c>
       <c r="C302" t="s">
         <v>789</v>
       </c>
@@ -7126,7 +7311,13 @@
         <v>843</v>
       </c>
     </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>802</v>
+      </c>
+      <c r="B303" t="s">
+        <v>831</v>
+      </c>
       <c r="C303" t="s">
         <v>790</v>
       </c>
@@ -7134,7 +7325,13 @@
         <v>845</v>
       </c>
     </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>802</v>
+      </c>
+      <c r="B304" t="s">
+        <v>831</v>
+      </c>
       <c r="C304" t="s">
         <v>791</v>
       </c>
@@ -7142,7 +7339,10 @@
         <v>844</v>
       </c>
     </row>
-    <row r="305" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>802</v>
+      </c>
       <c r="B305" t="s">
         <v>792</v>
       </c>
@@ -7153,7 +7353,13 @@
         <v>846</v>
       </c>
     </row>
-    <row r="306" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>802</v>
+      </c>
+      <c r="B306" t="s">
+        <v>792</v>
+      </c>
       <c r="C306" t="s">
         <v>287</v>
       </c>
@@ -7161,7 +7367,13 @@
         <v>847</v>
       </c>
     </row>
-    <row r="307" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>802</v>
+      </c>
+      <c r="B307" t="s">
+        <v>792</v>
+      </c>
       <c r="C307" t="s">
         <v>291</v>
       </c>
@@ -7169,7 +7381,13 @@
         <v>848</v>
       </c>
     </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>802</v>
+      </c>
+      <c r="B308" t="s">
+        <v>792</v>
+      </c>
       <c r="C308" t="s">
         <v>295</v>
       </c>
@@ -7177,7 +7395,13 @@
         <v>849</v>
       </c>
     </row>
-    <row r="309" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>802</v>
+      </c>
+      <c r="B309" t="s">
+        <v>792</v>
+      </c>
       <c r="C309" t="s">
         <v>794</v>
       </c>
@@ -7185,7 +7409,10 @@
         <v>850</v>
       </c>
     </row>
-    <row r="310" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>802</v>
+      </c>
       <c r="B310" t="s">
         <v>796</v>
       </c>
@@ -7196,7 +7423,13 @@
         <v>851</v>
       </c>
     </row>
-    <row r="311" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>802</v>
+      </c>
+      <c r="B311" t="s">
+        <v>796</v>
+      </c>
       <c r="C311" t="s">
         <v>300</v>
       </c>
@@ -7204,15 +7437,27 @@
         <v>852</v>
       </c>
     </row>
-    <row r="312" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C312" s="9" t="s">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>802</v>
+      </c>
+      <c r="B312" t="s">
+        <v>796</v>
+      </c>
+      <c r="C312" t="s">
         <v>303</v>
       </c>
       <c r="D312" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="313" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>802</v>
+      </c>
+      <c r="B313" t="s">
+        <v>796</v>
+      </c>
       <c r="C313" t="s">
         <v>306</v>
       </c>
@@ -7220,7 +7465,13 @@
         <v>854</v>
       </c>
     </row>
-    <row r="314" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>802</v>
+      </c>
+      <c r="B314" t="s">
+        <v>796</v>
+      </c>
       <c r="C314" t="s">
         <v>310</v>
       </c>
@@ -7228,18 +7479,24 @@
         <v>855</v>
       </c>
     </row>
-    <row r="315" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B315" s="9" t="s">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>802</v>
+      </c>
+      <c r="B315" t="s">
         <v>797</v>
       </c>
-      <c r="C315" s="9" t="s">
+      <c r="C315" t="s">
         <v>797</v>
       </c>
       <c r="D315" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="316" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>802</v>
+      </c>
       <c r="B316" t="s">
         <v>798</v>
       </c>
@@ -7250,7 +7507,13 @@
         <v>857</v>
       </c>
     </row>
-    <row r="317" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>802</v>
+      </c>
+      <c r="B317" t="s">
+        <v>798</v>
+      </c>
       <c r="C317" t="s">
         <v>319</v>
       </c>
@@ -7258,7 +7521,13 @@
         <v>858</v>
       </c>
     </row>
-    <row r="318" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>802</v>
+      </c>
+      <c r="B318" t="s">
+        <v>798</v>
+      </c>
       <c r="C318" t="s">
         <v>799</v>
       </c>
@@ -7446,7 +7715,7 @@
       <c r="C10" t="s">
         <v>302</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" t="s">
         <v>303</v>
       </c>
     </row>
@@ -8908,7 +9177,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>149</v>
       </c>
       <c r="B20" t="s">

</xml_diff>